<commit_message>
added all basic functions
</commit_message>
<xml_diff>
--- a/Tracker_enc.xlsx
+++ b/Tracker_enc.xlsx
@@ -385,7 +385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,28 +422,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>3445</t>
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44105</v>
+        <v>43466</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>43833</v>
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>43569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>